<commit_message>
add page transition file
</commit_message>
<xml_diff>
--- a/other/sample/web/151114 Page transition.xlsx
+++ b/other/sample/web/151114 Page transition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="4060" windowWidth="25520" windowHeight="11480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="page transition" sheetId="1" r:id="rId1"/>
@@ -4653,7 +4653,7 @@
   <dimension ref="A2:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -4721,7 +4721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B44"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>